<commit_message>
revisi buku tesis plus program
</commit_message>
<xml_diff>
--- a/data/rekap data 2019.xlsx
+++ b/data/rekap data 2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\bimbingan\catatanbimbingan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D299FCBF-16EC-40AD-90CB-832A455B3FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2F719-1613-441F-974A-D94194391DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5AF46FB8-2962-493F-8743-1EA874850232}"/>
   </bookViews>
@@ -150,10 +150,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76F216C-D313-4547-BA85-55A1A79F2B0A}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:M45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,31 +483,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -625,31 +625,31 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -746,21 +746,21 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -811,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -829,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="H24">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J24">
         <v>3</v>
@@ -848,7 +848,7 @@
       </c>
       <c r="N24">
         <f>SUM(B24:M24)</f>
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -923,11 +923,11 @@
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>86.36363636363636</v>
+        <v>85.714285714285708</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>68.75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
@@ -947,7 +947,7 @@
       </c>
       <c r="N26">
         <f>N24/(N24+N25)*100</f>
-        <v>73.831775700934571</v>
+        <v>73.076923076923066</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -999,13 +999,13 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -1014,7 +1014,7 @@
         <v>7</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -1023,20 +1023,20 @@
         <v>6</v>
       </c>
       <c r="J29">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N29">
         <f>SUM(B29:M29)</f>
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="Q29" t="s">
         <v>2</v>
@@ -1080,18 +1080,18 @@
         <v>2</v>
       </c>
       <c r="M30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N30">
         <f>SUM(B30:M30)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q30" t="s">
         <v>5</v>
       </c>
       <c r="R30">
         <f>N24+N29+N34</f>
-        <v>306</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
-        <v>83.333333333333343</v>
+        <v>75</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>76.923076923076934</v>
+        <v>72.727272727272734</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
@@ -1129,36 +1129,36 @@
       </c>
       <c r="J31">
         <f t="shared" si="1"/>
-        <v>56.521739130434781</v>
+        <v>50</v>
       </c>
       <c r="K31">
         <f t="shared" si="1"/>
-        <v>71.428571428571431</v>
+        <v>69.230769230769226</v>
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>71.428571428571431</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="M31">
         <f t="shared" si="1"/>
-        <v>57.142857142857139</v>
+        <v>20</v>
       </c>
       <c r="N31">
         <f t="shared" si="1"/>
-        <v>72.093023255813947</v>
+        <v>68.103448275862064</v>
       </c>
       <c r="Q31" t="s">
         <v>6</v>
       </c>
       <c r="R31">
         <f>N25+N30+N35</f>
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R32">
         <f>R30/(R30+R31)*100</f>
-        <v>73.205741626794264</v>
+        <v>71.571072319202003</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -1243,11 +1243,11 @@
         <v>5</v>
       </c>
       <c r="M34">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N34">
         <f>SUM(B34:M34)</f>
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -1288,11 +1288,11 @@
         <v>3</v>
       </c>
       <c r="M35">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N35">
         <f>SUM(B35:M35)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -1342,11 +1342,11 @@
       </c>
       <c r="M36">
         <f t="shared" si="2"/>
-        <v>66.666666666666657</v>
+        <v>58.82352941176471</v>
       </c>
       <c r="N36">
         <f t="shared" si="2"/>
-        <v>73.626373626373635</v>
+        <v>72.928176795580114</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -1360,15 +1360,15 @@
       </c>
       <c r="B39">
         <f>B24+B29+B34</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <f t="shared" ref="C39:M39" si="3">C24+C29+C34</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E39">
         <f t="shared" si="3"/>
@@ -1380,31 +1380,31 @@
       </c>
       <c r="G39">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H39">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I39">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J39">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K39">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L39">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M39">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="M40">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -1471,51 +1471,51 @@
       </c>
       <c r="B43">
         <f>B39</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C43">
         <f>B43+C39</f>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D43">
         <f t="shared" ref="D43:M43" si="5">C43+D39</f>
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E43">
         <f t="shared" si="5"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F43">
         <f t="shared" si="5"/>
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G43">
         <f t="shared" si="5"/>
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H43">
         <f t="shared" si="5"/>
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I43">
         <f t="shared" si="5"/>
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="J43">
         <f t="shared" si="5"/>
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="L43">
         <f t="shared" si="5"/>
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="M43">
         <f t="shared" si="5"/>
-        <v>306</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -1568,57 +1568,57 @@
       </c>
       <c r="M44">
         <f t="shared" si="6"/>
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <f>B43/(B43+B44)*100</f>
         <v>100</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <f t="shared" ref="C45:M45" si="7">C43/(C43+C44)*100</f>
-        <v>97.61904761904762</v>
-      </c>
-      <c r="D45" s="3">
+        <v>97.435897435897431</v>
+      </c>
+      <c r="D45" s="2">
         <f t="shared" si="7"/>
-        <v>94.20289855072464</v>
-      </c>
-      <c r="E45" s="3">
+        <v>93.75</v>
+      </c>
+      <c r="E45" s="2">
         <f t="shared" si="7"/>
-        <v>89.247311827956992</v>
-      </c>
-      <c r="F45" s="3">
+        <v>88.63636363636364</v>
+      </c>
+      <c r="F45" s="2">
         <f t="shared" si="7"/>
-        <v>86.99186991869918</v>
-      </c>
-      <c r="G45" s="3">
+        <v>86.440677966101703</v>
+      </c>
+      <c r="G45" s="2">
         <f t="shared" si="7"/>
-        <v>85.98726114649682</v>
-      </c>
-      <c r="H45" s="3">
+        <v>85.333333333333343</v>
+      </c>
+      <c r="H45" s="2">
         <f t="shared" si="7"/>
-        <v>85.643564356435647</v>
-      </c>
-      <c r="I45" s="3">
+        <v>85.051546391752581</v>
+      </c>
+      <c r="I45" s="2">
         <f t="shared" si="7"/>
-        <v>82.608695652173907</v>
-      </c>
-      <c r="J45" s="3">
+        <v>81.967213114754102</v>
+      </c>
+      <c r="J45" s="2">
         <f t="shared" si="7"/>
-        <v>74.08536585365853</v>
-      </c>
-      <c r="K45" s="3">
+        <v>73.101265822784811</v>
+      </c>
+      <c r="K45" s="2">
         <f t="shared" si="7"/>
-        <v>74.794520547945211</v>
-      </c>
-      <c r="L45" s="3">
+        <v>73.86363636363636</v>
+      </c>
+      <c r="L45" s="2">
         <f t="shared" si="7"/>
-        <v>74.418604651162795</v>
-      </c>
-      <c r="M45" s="3">
+        <v>73.458445040214485</v>
+      </c>
+      <c r="M45" s="2">
         <f t="shared" si="7"/>
-        <v>73.205741626794264</v>
+        <v>71.571072319202003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>